<commit_message>
- Add xlsx data.
</commit_message>
<xml_diff>
--- a/Doc/Catalog.xlsx
+++ b/Doc/Catalog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -48,163 +48,199 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>生物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>军事</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>企业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>市场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旅游</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>财经</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房产</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ParentName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Society</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Traffic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Good</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tech</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>健康</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Good|Tech</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Internet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Organ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Military</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>House</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>City</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Travel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Video</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>科技</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生物</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>军事</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>企业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>市场</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>股票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>天气</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>城市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>旅游</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>游戏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>财经</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>房产</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ParentName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Society</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Traffic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Car</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tech</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>健康</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good|Tech</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Internet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Organ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Military</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>House</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Company</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Market</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weather</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>City</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Travel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Game</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Video</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Health</t>
+    <t>电信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教育</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Woman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗教</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Religion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sports</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -556,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -575,12 +611,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -588,7 +624,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -596,15 +632,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -612,7 +648,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -620,15 +656,15 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -636,93 +672,96 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -730,34 +769,66 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>